<commit_message>
se realizo todas las preguntas
</commit_message>
<xml_diff>
--- a/2015-2016/PRE_PRO/pasantes/Victor Pua/2015/junio/SEGUIMIENTO Y CONTRO DE PRACTICAS Y PASANTIAS_15_19_junio.xlsx
+++ b/2015-2016/PRE_PRO/pasantes/Victor Pua/2015/junio/SEGUIMIENTO Y CONTRO DE PRACTICAS Y PASANTIAS_15_19_junio.xlsx
@@ -15,19 +15,21 @@
     <sheet name="VISITAS INSTITUCIONES-COMUNIDAD" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'VISITAS INSTITUCIONES-COMUNIDAD'!$A$1:$I$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'SUPERVISIÓN IN-SITU'!$A$1:$L$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'VISITAS INSTITUCIONES-COMUNIDAD'!$A$1:$I$22</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'VISITAS INSTITUCIONES-COMUNIDAD'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'VISITAS INSTITUCIONES-COMUNIDAD'!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
   <si>
     <t>UNIVERSIDAD TÉCNICA DE MACHALA</t>
   </si>
@@ -106,7 +108,19 @@
     </r>
   </si>
   <si>
-    <t>MES: Junio</t>
+    <r>
+      <t xml:space="preserve">MES: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Junio</t>
+    </r>
   </si>
   <si>
     <t>FECHA  DE VISITA</t>
@@ -146,26 +160,14 @@
 INSTITUCIONAL</t>
   </si>
   <si>
-    <t>Serrano Robles Danessa</t>
-  </si>
-  <si>
-    <t>0706911328</t>
-  </si>
-  <si>
-    <t>5 Paralelo A</t>
-  </si>
-  <si>
-    <t>Universidad Tecnica de 
-Machala</t>
-  </si>
-  <si>
-    <t>Econ. Gonzales Illescas Mayiya</t>
-  </si>
-  <si>
-    <t>Redaccion de Oficios
-Sistematizacion de Syllabus
-Copias de evaluacion, para el Subdecanato
-</t>
+    <t>Victor Hugo Pua Jurado</t>
+  </si>
+  <si>
+    <t>Paralelo A</t>
+  </si>
+  <si>
+    <t>Comercial y Fertilizantes 
+Mar Y Sierra</t>
   </si>
   <si>
     <t>_________________________________________________________</t>
@@ -174,9 +176,6 @@
     <t>TUTOR DE PRÁCTICAS PRE-PROFESIONALES Y PASANTÍAS</t>
   </si>
   <si>
-    <t>                                                                                                    UNIDAD ACADÉMICA DE CIENCIAS EMPRESARIALES</t>
-  </si>
-  <si>
     <t>PRÁCTICAS PRE-PROFESIONALES Y PASANTÍAS</t>
   </si>
   <si>
@@ -190,6 +189,9 @@
   </si>
   <si>
     <t>Del 01 al 05 de junio del 2015</t>
+  </si>
+  <si>
+    <t>MES: Junio</t>
   </si>
   <si>
     <t>FECHA</t>
@@ -215,6 +217,12 @@
   </si>
   <si>
     <t>USUARIO</t>
+  </si>
+  <si>
+    <t>Serrano Robles Danessa</t>
+  </si>
+  <si>
+    <t>0706911328</t>
   </si>
   <si>
     <t>Coordinacion de Comercio 
@@ -288,7 +296,7 @@
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -374,13 +382,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <u val="single"/>
       <sz val="18"/>
@@ -412,8 +413,22 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -447,7 +462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -512,6 +527,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
       <top/>
@@ -548,7 +570,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -617,15 +639,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,7 +655,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,6 +695,74 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,71 +775,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,11 +811,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -781,7 +827,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -851,15 +897,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1330200</xdr:colOff>
+      <xdr:colOff>1357200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1938960</xdr:colOff>
+      <xdr:colOff>1965600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -874,8 +920,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7071840" y="10440"/>
-          <a:ext cx="608760" cy="532440"/>
+          <a:off x="7098840" y="1440"/>
+          <a:ext cx="608400" cy="532080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -894,16 +940,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>628200</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>767880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>267840</xdr:rowOff>
+      <xdr:rowOff>272520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1390680</xdr:colOff>
+      <xdr:colOff>628200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -918,8 +964,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4019040" y="267840"/>
-          <a:ext cx="762480" cy="822960"/>
+          <a:off x="3256920" y="272520"/>
+          <a:ext cx="762120" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -939,15 +985,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>409680</xdr:colOff>
+      <xdr:colOff>436680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>885240</xdr:colOff>
+      <xdr:colOff>911880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -962,8 +1008,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4004280" y="144000"/>
-          <a:ext cx="475560" cy="761400"/>
+          <a:off x="4031280" y="135000"/>
+          <a:ext cx="475200" cy="761040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -983,15 +1029,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>396720</xdr:colOff>
+      <xdr:colOff>423720</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>894600</xdr:colOff>
+      <xdr:colOff>921240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1006,8 +1052,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3432600" y="144000"/>
-          <a:ext cx="497880" cy="766080"/>
+          <a:off x="3459600" y="135000"/>
+          <a:ext cx="497520" cy="765720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1027,15 +1073,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1165680</xdr:colOff>
+      <xdr:colOff>1192680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>277200</xdr:rowOff>
+      <xdr:rowOff>268200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2009880</xdr:colOff>
+      <xdr:colOff>2036520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1050,8 +1096,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4519080" y="277200"/>
-          <a:ext cx="844200" cy="829440"/>
+          <a:off x="4546080" y="268200"/>
+          <a:ext cx="843840" cy="829080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1324,10 +1370,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1442,7 +1488,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
@@ -1571,209 +1617,99 @@
     </row>
     <row r="12" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="n">
-        <v>42160</v>
+        <v>42167</v>
       </c>
       <c r="B12" s="32" t="n">
-        <v>0.583333333333333</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C12" s="32" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="8" t="s">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+    </row>
+    <row r="13" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-    </row>
-    <row r="25" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A1:L1"/>
@@ -1788,8 +1724,8 @@
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.236111111111111" right="0.196527777777778" top="0.39375" bottom="0.511805555555555" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1863,24 +1799,24 @@
       <c r="H3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="A4" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1891,20 +1827,20 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1925,78 +1861,78 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+    </row>
+    <row r="11" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38" t="s">
+      <c r="B11" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="C11" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="s">
+      <c r="D11" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="E11" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="F11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="G11" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="H11" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="I11" s="47"/>
+    </row>
+    <row r="12" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="48" t="n">
+        <v>42160</v>
+      </c>
+      <c r="B12" s="49" t="n">
+        <v>0.611111111111111</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="D12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="42" t="s">
+      <c r="E12" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="44"/>
-    </row>
-    <row r="12" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="n">
-        <v>42160</v>
-      </c>
-      <c r="B12" s="32" t="n">
-        <v>0.611111111111111</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="33" t="s">
+      <c r="F12" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -2102,30 +2038,30 @@
       <c r="H22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
+      <c r="A23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
     </row>
     <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2232,50 +2168,50 @@
       <c r="J3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="A4" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
+      <c r="A5" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -2288,16 +2224,16 @@
       <c r="J7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
@@ -2306,58 +2242,58 @@
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="49" t="s">
+      <c r="E9" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="56"/>
+      <c r="H9" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="F11" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="52" t="s">
+      <c r="G11" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="H11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="I11" s="30" t="s">
         <v>67</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>34</v>
@@ -2496,32 +2432,32 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
+      <c r="A23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
     </row>
     <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
+      <c r="A24" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2594,40 +2530,40 @@
       <c r="L1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
       <c r="J2" s="15"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="14"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2643,7 +2579,7 @@
     </row>
     <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2658,17 +2594,17 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="A6" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -2709,22 +2645,22 @@
         <v>25</v>
       </c>
       <c r="D9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="F9" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="G9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="80.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2827,30 +2763,30 @@
       <c r="I18" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="A20" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
     </row>
     <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>